<commit_message>
Ready for the run of LR 1-6 with time limit of 5800 to check the tests of 600_05
</commit_message>
<xml_diff>
--- a/Code/SampleRun_Environment_Solar/100Scens/100_Naive_CI.xlsx
+++ b/Code/SampleRun_Environment_Solar/100Scens/100_Naive_CI.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Dokumente\A_Uni\HiWi\ArticleSubgradient\Code\SampleRun_Environment_Solar\100Scens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{7842F81F-B3FC-42EF-B1BE-580A6B13F21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1AC603-ACCC-49C6-B5EB-4AB5D0A15BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,7 +453,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F481"/>
   <sheetViews>
     <sheetView topLeftCell="A463" workbookViewId="0">
@@ -8896,11 +8896,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9478,8 +9478,8 @@
         <v>9</v>
       </c>
       <c r="M19" s="2">
-        <f>AVERAGE(D42:D45,D47:D57,D59:D61)</f>
-        <v>2.4888888888888893E-4</v>
+        <f>AVERAGE(D42:D61)</f>
+        <v>2.6049999999999999E-4</v>
       </c>
       <c r="O19" t="s">
         <v>10</v>
@@ -9524,11 +9524,11 @@
       </c>
       <c r="P20" s="3">
         <f>M19-1.96*M23/(SQRT(20))</f>
-        <v>8.337562866892354E-5</v>
+        <v>9.4827963795938097E-5</v>
       </c>
       <c r="Q20" s="3">
         <f>M19+1.96*M23/(SQRT(20))</f>
-        <v>4.144021491088543E-4</v>
+        <v>4.2617203620406188E-4</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
@@ -9615,8 +9615,8 @@
         <v>12</v>
       </c>
       <c r="M23">
-        <f>_xlfn.STDEV.P(D42:D45,D47:D57,D59:D61)</f>
-        <v>3.7765193982597389E-4</v>
+        <f>_xlfn.STDEV.P(D42:D61)</f>
+        <v>3.7801421930927411E-4</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Test run for new main_for_lr gams scripts with the query if BBP holds with equality and extraction of upper bound LR included
</commit_message>
<xml_diff>
--- a/Code/SampleRun_Environment_Solar/100Scens/100_Naive_CI.xlsx
+++ b/Code/SampleRun_Environment_Solar/100Scens/100_Naive_CI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Dokumente\A_Uni\HiWi\ArticleSubgradient\Code\SampleRun_Environment_Solar\100Scens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1AC603-ACCC-49C6-B5EB-4AB5D0A15BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63309315-2093-42F6-B989-4A49DCA636FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
   <si>
     <t>Instance</t>
   </si>
@@ -81,6 +84,15 @@
   </si>
   <si>
     <t>Time:</t>
+  </si>
+  <si>
+    <t>95% normal</t>
+  </si>
+  <si>
+    <t>t dist 95%</t>
+  </si>
+  <si>
+    <t>t dist 97.5%</t>
   </si>
 </sst>
 </file>
@@ -132,13 +144,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -155,6 +168,1669 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>0.01</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$E$2:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>269.25283000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>278.53877</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>273.90879000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>273.49889000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>273.26862999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>268.74007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>280.63983999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>277.79477000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>268.85066</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>274.24653999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>276.42693000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>272.33364</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>270.61401000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>274.54435999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>267.64940000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>268.45136000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>269.93166000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>275.64729999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>278.13220999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>279.69051000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-259D-4660-8DE0-34BEA2DBBF9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>0.03</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="24130" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$E$22:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>282.08202999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>280.04689000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>276.99113</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>277.99176</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>280.17264999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>271.73601000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>282.49918000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>280.98261000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>277.43299999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>280.60424999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>277.64512000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>276.98005999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>281.84093000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>280.65692000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>278.14305000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>279.45004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>276.21485000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>277.70031</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>280.24694</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>281.43982999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-259D-4660-8DE0-34BEA2DBBF9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>0.05</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22860" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$E$42:$E$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>283.13659999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>280.98160000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>279.61932999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>280.75729000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>283.78976999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>282.27202</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>284.07028000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>282.69468000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>279.49662000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>282.03235000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>281.29417000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>279.60034999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>283.02118000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>281.86711000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>282.66964999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>280.49160000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>279.18200999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>281.53742999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>281.53131999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>282.32378</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-259D-4660-8DE0-34BEA2DBBF9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>0.07</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$E$62:$E$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>284.47788000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>283.99196999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>280.91435999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>283.58837</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>285.01670999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>284.15595000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>285.45290999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>283.87349</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>280.90575000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>284.98086999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>283.32538</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>282.44033000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>284.90622999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>283.28921000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>285.58792999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>281.35509000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>283.78881999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>282.76985999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>282.0763</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>283.33836000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-259D-4660-8DE0-34BEA2DBBF9F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="734219999"/>
+        <c:axId val="734219167"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="734219999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="734219167"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="734219167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="265"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="734219999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>549275</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DD34E8B-CDA0-4464-9DB6-652212A0783A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Tabelle1"/>
+      <sheetName val="Tabelle2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="E2">
+            <v>246.57187999999999</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="E3">
+            <v>252.31788</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="E4">
+            <v>241.72673</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5">
+            <v>248.41552999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="E6">
+            <v>244.96548000000001</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="E7">
+            <v>242.33189999999999</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="E8">
+            <v>247.05856</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="E9">
+            <v>244.36434</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="E10">
+            <v>226.78341</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="E11">
+            <v>242.86644000000001</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="E12">
+            <v>243.84789000000001</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="E13">
+            <v>246.25400999999999</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="E14">
+            <v>242.58036999999999</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="E15">
+            <v>242.59375</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="E16">
+            <v>237.65900999999999</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="E17">
+            <v>243.28272000000001</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="E18">
+            <v>249.03632999999999</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="E19">
+            <v>243.27918</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="E20">
+            <v>247.50851</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="E21">
+            <v>251.81213</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="E22">
+            <v>232.13278</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="E23">
+            <v>251.53009</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="E24">
+            <v>242.60290000000001</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="E25">
+            <v>248.46988999999999</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="E26">
+            <v>244.57126</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="E27">
+            <v>240.90254999999999</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="E28">
+            <v>247.90880000000001</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="E29">
+            <v>244.49700000000001</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="E30">
+            <v>226.90988999999999</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="E31">
+            <v>242.15585999999999</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="E32">
+            <v>244.10871</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="E33">
+            <v>245.49118999999999</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="E34">
+            <v>242.52088000000001</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="E35">
+            <v>241.27199999999999</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="E36">
+            <v>236.15630999999999</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="E37">
+            <v>243.37649999999999</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="E38">
+            <v>247.95142000000001</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="E39">
+            <v>241.87454</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="E40">
+            <v>234.69932</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="E41">
+            <v>243.59105</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="E42">
+            <v>232.29670999999999</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="E43">
+            <v>251.70405</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="E44">
+            <v>243.69188</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="E45">
+            <v>245.28541000000001</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="E46">
+            <v>244.30515</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="E47">
+            <v>240.90186</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="E48">
+            <v>247.34291999999999</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="E49">
+            <v>248.4933</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="E50">
+            <v>226.73808</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="E51">
+            <v>242.36433</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="E52">
+            <v>243.53668999999999</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="E53">
+            <v>245.39230000000001</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="E54">
+            <v>242.28900999999999</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="E55">
+            <v>237.57219000000001</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="E56">
+            <v>235.30489</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="E57">
+            <v>242.20921000000001</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="E58">
+            <v>248.03596999999999</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="E59">
+            <v>241.14474999999999</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="E60">
+            <v>236.88746</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="E61">
+            <v>243.64015000000001</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="E62">
+            <v>246.97856999999999</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="E63">
+            <v>252.13225</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="E64">
+            <v>242.16369</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="E65">
+            <v>245.78738999999999</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="E66">
+            <v>242.63132999999999</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="E67">
+            <v>242.97719000000001</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="E68">
+            <v>247.00099</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="E69">
+            <v>244.70248000000001</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="E70">
+            <v>226.67839000000001</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="E71">
+            <v>242.35542000000001</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="E72">
+            <v>241.16963999999999</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="E73">
+            <v>245.03030000000001</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="E74">
+            <v>242.70593</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="E75">
+            <v>239.19291000000001</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="E76">
+            <v>240.72725</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="E77">
+            <v>243.13899000000001</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="E78">
+            <v>247.89068</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="E79">
+            <v>241.14474999999999</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="E80">
+            <v>234.94042999999999</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="E81">
+            <v>243.74502000000001</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8897,15 +10573,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:Y81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8927,8 +10603,17 @@
       <c r="L1" s="1">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8960,8 +10645,20 @@
       <c r="Q2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="S2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>10</v>
       </c>
@@ -8992,14 +10689,36 @@
       </c>
       <c r="P3">
         <f>M2+(-1.96)*M6/(SQRT(20))</f>
-        <v>271.87189035932653</v>
+        <v>271.82678757208907</v>
       </c>
       <c r="Q3">
         <f>M2+1.96*M6/(SQRT(20))</f>
-        <v>275.34422664067353</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>275.38932942791098</v>
+      </c>
+      <c r="S3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3">
+        <f>M2+(-$H$10)*M6/(SQRT(20))</f>
+        <v>271.70589375533888</v>
+      </c>
+      <c r="U3">
+        <f>M2+$H$10*M6/(SQRT(20))</f>
+        <v>275.51022324466118</v>
+      </c>
+      <c r="W3" t="s">
+        <v>10</v>
+      </c>
+      <c r="X3">
+        <f>M2+(-$H$11)*M6/(SQRT(20))</f>
+        <v>271.39651956972875</v>
+      </c>
+      <c r="Y3">
+        <f>M2+($H$11)*M6/(SQRT(20))</f>
+        <v>275.8195974302713</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11</v>
       </c>
@@ -9030,14 +10749,14 @@
       </c>
       <c r="P4" s="3">
         <f>M3-1.96*M7/(SQRT(20))</f>
-        <v>-2.5849879369427173E-5</v>
+        <v>-2.8651641508027533E-5</v>
       </c>
       <c r="Q4" s="3">
         <f>M3+1.96*M7/(SQRT(20))</f>
-        <v>1.8984987936942717E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1.9265164150802754E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>12</v>
       </c>
@@ -9064,14 +10783,14 @@
       </c>
       <c r="P5">
         <f>M4-1.96*M8/(SQRT(20))</f>
-        <v>56.449960219756917</v>
+        <v>56.107044938807725</v>
       </c>
       <c r="Q5">
         <f>M4+1.96*M8/(SQRT(20))</f>
-        <v>82.850039780243094</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>83.192955061192293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>13</v>
       </c>
@@ -9094,11 +10813,11 @@
         <v>10</v>
       </c>
       <c r="M6">
-        <f>_xlfn.STDEV.P(E2:E21)</f>
-        <v>3.961418349913667</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <f>_xlfn.STDEV.S(E2:E21)</f>
+        <v>4.0643294705643145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>14</v>
       </c>
@@ -9121,11 +10840,11 @@
         <v>12</v>
       </c>
       <c r="M7">
-        <f>_xlfn.STDEV.P(D2:D21)</f>
-        <v>2.460812873828483E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <f>_xlfn.STDEV.S(D2:D21)</f>
+        <v>2.5247407370804789E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>15</v>
       </c>
@@ -9148,11 +10867,11 @@
         <v>14</v>
       </c>
       <c r="M8">
-        <f>_xlfn.STDEV.P(F2:F21)</f>
-        <v>30.118557402372378</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <f>_xlfn.STDEV.S(F2:F21)</f>
+        <v>30.900987890868134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>16</v>
       </c>
@@ -9175,7 +10894,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>17</v>
       </c>
@@ -9193,6 +10912,13 @@
       </c>
       <c r="F10">
         <v>54</v>
+      </c>
+      <c r="H10">
+        <f>_xlfn.T.INV(0.975,19)</f>
+        <v>2.0930240544083087</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.95</v>
       </c>
       <c r="L10" t="s">
         <v>6</v>
@@ -9208,7 +10934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>18</v>
       </c>
@@ -9226,6 +10952,13 @@
       </c>
       <c r="F11">
         <v>82</v>
+      </c>
+      <c r="H11">
+        <f>_xlfn.T.INV(0.9875,19)</f>
+        <v>2.4334402113749714</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.97499999999999998</v>
       </c>
       <c r="L11" t="s">
         <v>9</v>
@@ -9239,14 +10972,22 @@
       </c>
       <c r="P11">
         <f>M10+(-1.96)*M14/(SQRT(20))</f>
-        <v>277.94467484935387</v>
+        <v>277.91614534124534</v>
       </c>
       <c r="Q11">
         <f>M10+1.96*M14/(SQRT(20))</f>
-        <v>280.14108115064619</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>280.16961065875472</v>
+      </c>
+      <c r="T11">
+        <f>M10+(-$H$10)*M14/(SQRT(20))</f>
+        <v>277.83967465425462</v>
+      </c>
+      <c r="U11">
+        <f>M10+$H$10*M14/(SQRT(20))</f>
+        <v>280.24608134574544</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>19</v>
       </c>
@@ -9277,14 +11018,14 @@
       </c>
       <c r="P12" s="3">
         <f>M11-1.96*M15/(SQRT(20))</f>
-        <v>9.1083060596875901E-5</v>
+        <v>8.7188465561532799E-5</v>
       </c>
       <c r="Q12" s="3">
         <f>M11+1.96*M15/(SQRT(20))</f>
-        <v>3.9091693940312413E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>3.9481153443846723E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2</v>
       </c>
@@ -9311,14 +11052,14 @@
       </c>
       <c r="P13">
         <f>M12-1.96*M16/(SQRT(20))</f>
-        <v>204.2295386341234</v>
+        <v>203.77698375527481</v>
       </c>
       <c r="Q13">
         <f>M12+1.96*M16/(SQRT(20))</f>
-        <v>239.07046136587661</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>239.5230162447252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>20</v>
       </c>
@@ -9341,11 +11082,11 @@
         <v>10</v>
       </c>
       <c r="M14">
-        <f>_xlfn.STDEV.P(E22:E41)</f>
-        <v>2.5057723448461919</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <f>_xlfn.STDEV.S(E22:E41)</f>
+        <v>2.5708681810658485</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3</v>
       </c>
@@ -9368,11 +11109,11 @@
         <v>12</v>
       </c>
       <c r="M15">
-        <f>_xlfn.STDEV.P(D22:D41)</f>
-        <v>3.4206578314704321E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <f>_xlfn.STDEV.S(D22:D41)</f>
+        <v>3.5095208849792109E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>4</v>
       </c>
@@ -9395,11 +11136,11 @@
         <v>14</v>
       </c>
       <c r="M16">
-        <f>_xlfn.STDEV.P(F22:F41)</f>
-        <v>39.748301850519347</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+        <f>_xlfn.STDEV.S(F22:F41)</f>
+        <v>40.780897230779154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>5</v>
       </c>
@@ -9422,7 +11163,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>6</v>
       </c>
@@ -9455,7 +11196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>7</v>
       </c>
@@ -9486,14 +11227,22 @@
       </c>
       <c r="P19">
         <f>M18+(-1.96)*M22/(SQRT(20))</f>
-        <v>281.00282116402582</v>
+        <v>280.98682795952266</v>
       </c>
       <c r="Q19">
         <f>M18+1.96*M22/(SQRT(20))</f>
-        <v>282.23409283597414</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+        <v>282.2500860404773</v>
+      </c>
+      <c r="T19">
+        <f>M18+(-$H$10)*M22/(SQRT(20))</f>
+        <v>280.94395966572353</v>
+      </c>
+      <c r="U19">
+        <f>M18+$H$10*M22/(SQRT(20))</f>
+        <v>282.29295433427643</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>8</v>
       </c>
@@ -9524,14 +11273,14 @@
       </c>
       <c r="P20" s="3">
         <f>M19-1.96*M23/(SQRT(20))</f>
-        <v>9.4827963795938097E-5</v>
+        <v>9.052407730876459E-5</v>
       </c>
       <c r="Q20" s="3">
         <f>M19+1.96*M23/(SQRT(20))</f>
-        <v>4.2617203620406188E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+        <v>4.3047592269123542E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>9</v>
       </c>
@@ -9558,14 +11307,14 @@
       </c>
       <c r="P21">
         <f>M20-1.96*M24/(SQRT(20))</f>
-        <v>389.55609240726619</v>
+        <v>388.7743022802041</v>
       </c>
       <c r="Q21">
         <f>M20+1.96*M24/(SQRT(20))</f>
-        <v>449.74390759273376</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+        <v>450.52569771979586</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -9588,11 +11337,11 @@
         <v>10</v>
       </c>
       <c r="M22">
-        <f>_xlfn.STDEV.P(E42:E61)</f>
-        <v>1.4046975292072676</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+        <f>_xlfn.STDEV.S(E42:E61)</f>
+        <v>1.4411892561941602</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>10</v>
       </c>
@@ -9615,11 +11364,11 @@
         <v>12</v>
       </c>
       <c r="M23">
-        <f>_xlfn.STDEV.P(D42:D61)</f>
-        <v>3.7801421930927411E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+        <f>_xlfn.STDEV.S(D42:D61)</f>
+        <v>3.8783440579168507E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>11</v>
       </c>
@@ -9642,11 +11391,11 @@
         <v>14</v>
       </c>
       <c r="M24">
-        <f>_xlfn.STDEV.P(F42:F61)</f>
-        <v>68.665329679540605</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+        <f>_xlfn.STDEV.S(F42:F61)</f>
+        <v>70.449141789998833</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>12</v>
       </c>
@@ -9669,7 +11418,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>13</v>
       </c>
@@ -9702,7 +11451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>14</v>
       </c>
@@ -9733,14 +11482,22 @@
       </c>
       <c r="P27">
         <f>M26+(-1.96)*M30/(SQRT(20))</f>
-        <v>282.90528837711508</v>
+        <v>282.88953250338307</v>
       </c>
       <c r="Q27">
         <f>M26+1.96*M30/(SQRT(20))</f>
-        <v>284.11828862288485</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+        <v>284.13404449661687</v>
+      </c>
+      <c r="T27">
+        <f>M26+(-$H$10)*M30/(SQRT(20))</f>
+        <v>282.84730035259236</v>
+      </c>
+      <c r="U27">
+        <f>M26+$H$10*M30/(SQRT(20))</f>
+        <v>284.17627664740758</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>15</v>
       </c>
@@ -9771,14 +11528,14 @@
       </c>
       <c r="P28" s="3">
         <f>M27-1.96*M31/(SQRT(20))</f>
-        <v>2.9384387038063856E-4</v>
+        <v>2.8872833569168791E-4</v>
       </c>
       <c r="Q28" s="3">
         <f>M27+1.96*M31/(SQRT(20))</f>
-        <v>6.6720876119830889E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+        <v>6.7232429588725954E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>16</v>
       </c>
@@ -9805,14 +11562,14 @@
       </c>
       <c r="P29">
         <f>M28-1.96*M32/(SQRT(20))</f>
-        <v>558.12311054209715</v>
+        <v>556.95208723685619</v>
       </c>
       <c r="Q29">
         <f>M28+1.96*M32/(SQRT(20))</f>
-        <v>648.27688945790294</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+        <v>649.4479127631439</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>17</v>
       </c>
@@ -9835,11 +11592,11 @@
         <v>10</v>
       </c>
       <c r="M30">
-        <f>_xlfn.STDEV.P(E62:E81)</f>
-        <v>1.3838525542169333</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+        <f>_xlfn.STDEV.S(E62:E81)</f>
+        <v>1.4198027631043206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>18</v>
       </c>
@@ -9862,11 +11619,11 @@
         <v>12</v>
       </c>
       <c r="M31">
-        <f>_xlfn.STDEV.P(D62:D75,D77:D81)</f>
-        <v>4.2595371238780502E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+        <f>_xlfn.STDEV.S(D62:D75,D77:D81)</f>
+        <v>4.3762583821000089E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>19</v>
       </c>
@@ -9889,8 +11646,8 @@
         <v>14</v>
       </c>
       <c r="M32">
-        <f>_xlfn.STDEV.P(F50:F69)</f>
-        <v>102.8520296348108</v>
+        <f>_xlfn.STDEV.S(F50:F69)</f>
+        <v>105.52395587333658</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -10875,5 +12632,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Prepared last run of 600 Wind Samples for 4200 time limit
</commit_message>
<xml_diff>
--- a/Code/SampleRun_Environment_Solar/100Scens/100_Naive_CI.xlsx
+++ b/Code/SampleRun_Environment_Solar/100Scens/100_Naive_CI.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Dokumente\A_Uni\HiWi\ArticleSubgradient\Code\SampleRun_Environment_Solar\100Scens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63309315-2093-42F6-B989-4A49DCA636FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9E762C-3262-49FF-9C17-53AB804160FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="18">
   <si>
     <t>Instance</t>
   </si>
@@ -1417,422 +1414,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Tabelle1"/>
-      <sheetName val="Tabelle2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="E2">
-            <v>246.57187999999999</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="E3">
-            <v>252.31788</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="E4">
-            <v>241.72673</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="E5">
-            <v>248.41552999999999</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="E6">
-            <v>244.96548000000001</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="E7">
-            <v>242.33189999999999</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="E8">
-            <v>247.05856</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9">
-            <v>244.36434</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>226.78341</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>242.86644000000001</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>243.84789000000001</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>246.25400999999999</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>242.58036999999999</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="E15">
-            <v>242.59375</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>237.65900999999999</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>243.28272000000001</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>249.03632999999999</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>243.27918</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>247.50851</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="E21">
-            <v>251.81213</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>232.13278</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>251.53009</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>242.60290000000001</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>248.46988999999999</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>244.57126</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="E27">
-            <v>240.90254999999999</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="E28">
-            <v>247.90880000000001</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29">
-            <v>244.49700000000001</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30">
-            <v>226.90988999999999</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31">
-            <v>242.15585999999999</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>244.10871</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>245.49118999999999</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="E34">
-            <v>242.52088000000001</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35">
-            <v>241.27199999999999</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36">
-            <v>236.15630999999999</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>243.37649999999999</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="E38">
-            <v>247.95142000000001</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39">
-            <v>241.87454</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="E40">
-            <v>234.69932</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="E41">
-            <v>243.59105</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="E42">
-            <v>232.29670999999999</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="E43">
-            <v>251.70405</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>243.69188</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>245.28541000000001</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="E46">
-            <v>244.30515</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>240.90186</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="E48">
-            <v>247.34291999999999</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49">
-            <v>248.4933</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>226.73808</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51">
-            <v>242.36433</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="E52">
-            <v>243.53668999999999</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="E53">
-            <v>245.39230000000001</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>242.28900999999999</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>237.57219000000001</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="E56">
-            <v>235.30489</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>242.20921000000001</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="E58">
-            <v>248.03596999999999</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="E59">
-            <v>241.14474999999999</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>236.88746</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>243.64015000000001</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>246.97856999999999</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>252.13225</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="E64">
-            <v>242.16369</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="E65">
-            <v>245.78738999999999</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="E66">
-            <v>242.63132999999999</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="E67">
-            <v>242.97719000000001</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="E68">
-            <v>247.00099</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="E69">
-            <v>244.70248000000001</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="E70">
-            <v>226.67839000000001</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="E71">
-            <v>242.35542000000001</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="E72">
-            <v>241.16963999999999</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="E73">
-            <v>245.03030000000001</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="E74">
-            <v>242.70593</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="E75">
-            <v>239.19291000000001</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="E76">
-            <v>240.72725</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="E77">
-            <v>243.13899000000001</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="E78">
-            <v>247.89068</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="E79">
-            <v>241.14474999999999</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="E80">
-            <v>234.94042999999999</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="E81">
-            <v>243.74502000000001</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -10576,10 +10157,13 @@
   <dimension ref="A1:Y81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="20" max="20" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -10755,6 +10339,17 @@
         <f>M3+1.96*M7/(SQRT(20))</f>
         <v>1.9265164150802754E-4</v>
       </c>
+      <c r="S4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4">
+        <f>M3+(-$H$10)*M7/(SQRT(20))</f>
+        <v>-3.6161503742891077E-5</v>
+      </c>
+      <c r="U4">
+        <f>M3+$H$10*M7/(SQRT(20))</f>
+        <v>2.0016150374289107E-4</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -10789,6 +10384,17 @@
         <f>M4+1.96*M8/(SQRT(20))</f>
         <v>83.192955061192293</v>
       </c>
+      <c r="S5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T5">
+        <f>M4+(-$H$10)*M8/(SQRT(20))</f>
+        <v>55.187892494466233</v>
+      </c>
+      <c r="U5">
+        <f>M4+$H$10*M8/(SQRT(20))</f>
+        <v>84.112107505533785</v>
+      </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -10978,6 +10584,9 @@
         <f>M10+1.96*M14/(SQRT(20))</f>
         <v>280.16961065875472</v>
       </c>
+      <c r="S11" t="s">
+        <v>10</v>
+      </c>
       <c r="T11">
         <f>M10+(-$H$10)*M14/(SQRT(20))</f>
         <v>277.83967465425462</v>
@@ -11024,6 +10633,17 @@
         <f>M11+1.96*M15/(SQRT(20))</f>
         <v>3.9481153443846723E-4</v>
       </c>
+      <c r="S12" t="s">
+        <v>12</v>
+      </c>
+      <c r="T12">
+        <f>M11+(-$H$10)*M15/(SQRT(20))</f>
+        <v>7.6749366619814375E-5</v>
+      </c>
+      <c r="U12">
+        <f>M11+$H$10*M15/(SQRT(20))</f>
+        <v>4.0525063338018566E-4</v>
+      </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -11058,6 +10678,17 @@
         <f>M12+1.96*M16/(SQRT(20))</f>
         <v>239.5230162447252</v>
       </c>
+      <c r="S13" t="s">
+        <v>14</v>
+      </c>
+      <c r="T13">
+        <f>M12+(-$H$10)*M16/(SQRT(20))</f>
+        <v>202.56395258926517</v>
+      </c>
+      <c r="U13">
+        <f>M12+$H$10*M16/(SQRT(20))</f>
+        <v>240.73604741073484</v>
+      </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -11233,6 +10864,9 @@
         <f>M18+1.96*M22/(SQRT(20))</f>
         <v>282.2500860404773</v>
       </c>
+      <c r="S19" t="s">
+        <v>10</v>
+      </c>
       <c r="T19">
         <f>M18+(-$H$10)*M22/(SQRT(20))</f>
         <v>280.94395966572353</v>
@@ -11279,6 +10913,17 @@
         <f>M19+1.96*M23/(SQRT(20))</f>
         <v>4.3047592269123542E-4</v>
       </c>
+      <c r="S20" t="s">
+        <v>12</v>
+      </c>
+      <c r="T20" s="3">
+        <f>M19+(-$H$10)*M23/(SQRT(20))</f>
+        <v>7.8987910784182266E-5</v>
+      </c>
+      <c r="U20" s="3">
+        <f>M19+$H$10*M23/(SQRT(20))</f>
+        <v>4.4201208921581771E-4</v>
+      </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
@@ -11313,6 +10958,17 @@
         <f>M20+1.96*M24/(SQRT(20))</f>
         <v>450.52569771979586</v>
       </c>
+      <c r="S21" t="s">
+        <v>14</v>
+      </c>
+      <c r="T21">
+        <f>M20+(-$H$10)*M24/(SQRT(20))</f>
+        <v>386.67878672236094</v>
+      </c>
+      <c r="U21">
+        <f>M20+$H$10*M24/(SQRT(20))</f>
+        <v>452.62121327763901</v>
+      </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22">
@@ -11488,6 +11144,9 @@
         <f>M26+1.96*M30/(SQRT(20))</f>
         <v>284.13404449661687</v>
       </c>
+      <c r="S27" t="s">
+        <v>10</v>
+      </c>
       <c r="T27">
         <f>M26+(-$H$10)*M30/(SQRT(20))</f>
         <v>282.84730035259236</v>
@@ -11534,6 +11193,17 @@
         <f>M27+1.96*M31/(SQRT(20))</f>
         <v>6.7232429588725954E-4</v>
       </c>
+      <c r="S28" t="s">
+        <v>12</v>
+      </c>
+      <c r="T28">
+        <f>M27+(-$H$10)*M31/(SQRT(20))</f>
+        <v>2.7571111888560036E-4</v>
+      </c>
+      <c r="U28">
+        <f>M27+$H$10*M31/(SQRT(20))</f>
+        <v>6.853415126933471E-4</v>
+      </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29">
@@ -11567,6 +11237,17 @@
       <c r="Q29">
         <f>M28+1.96*M32/(SQRT(20))</f>
         <v>649.4479127631439</v>
+      </c>
+      <c r="S29" t="s">
+        <v>14</v>
+      </c>
+      <c r="T29">
+        <f>M28+(-$H$10)*M32/(SQRT(20))</f>
+        <v>553.81326842885869</v>
+      </c>
+      <c r="U29">
+        <f>M28+$H$10*M32/(SQRT(20))</f>
+        <v>652.5867315711414</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>